<commit_message>
rozpisane rozjazdy na 08.01 i 0901
</commit_message>
<xml_diff>
--- a/rozliczenie zbiorcze1.xlsx
+++ b/rozliczenie zbiorcze1.xlsx
@@ -9,17 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10910" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pakiet_Zlecen_WTA_2019_01_03s.s" sheetId="1" r:id="rId1"/>
+    <sheet name="rozjazdy 08.01" sheetId="2" r:id="rId2"/>
+    <sheet name="rozjazdy 09.01" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="114">
   <si>
     <t>MONIKA ŁUCZAK</t>
   </si>
@@ -33,9 +35,6 @@
     <t>17457.38</t>
   </si>
   <si>
-    <t>Jan 10 201</t>
-  </si>
-  <si>
     <t>ANNA WARKOCZYŃSKA</t>
   </si>
   <si>
@@ -352,6 +351,18 @@
   </si>
   <si>
     <t>pod borkiem</t>
+  </si>
+  <si>
+    <t>za miliczem</t>
+  </si>
+  <si>
+    <t>za kostomlotami</t>
+  </si>
+  <si>
+    <t>iedzy lagiewnikami a strzelinem</t>
+  </si>
+  <si>
+    <t>gm. Katy wroclawskie</t>
   </si>
 </sst>
 </file>
@@ -708,7 +719,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -823,6 +834,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -868,7 +894,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -887,6 +913,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1211,13 +1255,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.6328125" bestFit="1" customWidth="1"/>
@@ -1228,94 +1272,94 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
       <c r="G1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1">
+        <v>82</v>
+      </c>
+      <c r="H1" s="9">
         <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2">
+        <v>82</v>
+      </c>
+      <c r="H2" s="12">
         <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H3">
+        <v>82</v>
+      </c>
+      <c r="H3" s="12">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H4">
+        <v>82</v>
+      </c>
+      <c r="H4" s="12">
         <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="5"/>
       <c r="G5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H5">
+        <v>82</v>
+      </c>
+      <c r="H5" s="12">
         <v>65</v>
       </c>
     </row>
@@ -1330,7 +1374,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -1339,9 +1383,9 @@
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H6">
+        <v>91</v>
+      </c>
+      <c r="H6" s="9">
         <v>40</v>
       </c>
     </row>
@@ -1350,24 +1394,24 @@
         <v>2657085</v>
       </c>
       <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
       <c r="G7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H7">
+        <v>91</v>
+      </c>
+      <c r="H7" s="12">
         <v>40</v>
       </c>
     </row>
@@ -1376,24 +1420,24 @@
         <v>2663720</v>
       </c>
       <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
       <c r="G8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H8">
+        <v>91</v>
+      </c>
+      <c r="H8" s="9">
         <v>40</v>
       </c>
     </row>
@@ -1402,24 +1446,24 @@
         <v>2949099</v>
       </c>
       <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
         <v>94</v>
       </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H9">
+      <c r="H9" s="9">
         <v>40</v>
       </c>
     </row>
@@ -1428,28 +1472,31 @@
         <v>2958822</v>
       </c>
       <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
         <v>96</v>
       </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="H10" s="12">
+        <v>70</v>
+      </c>
+      <c r="J10" t="s">
         <v>97</v>
       </c>
-      <c r="H10">
-        <v>60</v>
-      </c>
-      <c r="J10" t="s">
-        <v>98</v>
+      <c r="K10" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -1457,25 +1504,28 @@
         <v>3037547</v>
       </c>
       <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="D11" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E11">
         <v>8382958</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>100</v>
-      </c>
-      <c r="H11">
+        <v>99</v>
+      </c>
+      <c r="H11" s="9">
         <v>40</v>
+      </c>
+      <c r="J11" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -1483,24 +1533,24 @@
         <v>3067160</v>
       </c>
       <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="E12" t="s">
         <v>26</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>27</v>
       </c>
-      <c r="F12" t="s">
-        <v>28</v>
-      </c>
       <c r="G12" t="s">
-        <v>100</v>
-      </c>
-      <c r="H12">
+        <v>99</v>
+      </c>
+      <c r="H12" s="9">
         <v>40</v>
       </c>
     </row>
@@ -1509,28 +1559,31 @@
         <v>3073191</v>
       </c>
       <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="E13" t="s">
         <v>31</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>32</v>
       </c>
-      <c r="F13" t="s">
-        <v>33</v>
-      </c>
       <c r="G13" t="s">
-        <v>100</v>
-      </c>
-      <c r="H13">
-        <v>60</v>
+        <v>99</v>
+      </c>
+      <c r="H13" s="9">
+        <v>70</v>
       </c>
       <c r="J13" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="K13" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -1538,28 +1591,28 @@
         <v>3074967</v>
       </c>
       <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="D14" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E14">
         <v>1755131</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K14">
         <v>104</v>
@@ -1570,24 +1623,24 @@
         <v>2955619</v>
       </c>
       <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="D15" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E15">
         <v>2181000</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>97</v>
-      </c>
-      <c r="H15">
+        <v>96</v>
+      </c>
+      <c r="H15" s="12">
         <v>40</v>
       </c>
     </row>
@@ -1596,28 +1649,28 @@
         <v>3037067</v>
       </c>
       <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="E16">
         <v>3458347</v>
       </c>
       <c r="F16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>100</v>
-      </c>
-      <c r="H16">
-        <v>60</v>
+        <v>99</v>
+      </c>
+      <c r="H16" s="12">
+        <v>70</v>
       </c>
       <c r="J16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K16">
         <v>55</v>
@@ -1628,25 +1681,25 @@
         <v>2951874</v>
       </c>
       <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="D17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>46</v>
       </c>
-      <c r="F17" t="s">
-        <v>47</v>
-      </c>
       <c r="G17" t="s">
-        <v>97</v>
-      </c>
-      <c r="H17">
-        <v>60</v>
+        <v>96</v>
+      </c>
+      <c r="H17" s="12">
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -1654,25 +1707,25 @@
         <v>2966414</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="E18">
         <v>3628938</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G18" t="s">
-        <v>97</v>
-      </c>
-      <c r="H18">
-        <v>60</v>
+        <v>96</v>
+      </c>
+      <c r="H18" s="12">
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -1680,24 +1733,24 @@
         <v>3266106</v>
       </c>
       <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>53</v>
       </c>
       <c r="E19">
         <v>3211863</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G19" t="s">
-        <v>107</v>
-      </c>
-      <c r="H19">
+        <v>106</v>
+      </c>
+      <c r="H19" s="9">
         <v>65</v>
       </c>
     </row>
@@ -1706,25 +1759,28 @@
         <v>3266289</v>
       </c>
       <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="D20" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="E20">
         <v>1929525</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G20" t="s">
-        <v>107</v>
-      </c>
-      <c r="H20">
+        <v>106</v>
+      </c>
+      <c r="H20" s="12">
         <v>65</v>
+      </c>
+      <c r="K20" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -1732,24 +1788,24 @@
         <v>3266324</v>
       </c>
       <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="D21" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="E21">
         <v>1603687</v>
       </c>
       <c r="F21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>107</v>
-      </c>
-      <c r="H21">
+        <v>106</v>
+      </c>
+      <c r="H21" s="9">
         <v>65</v>
       </c>
     </row>
@@ -1758,21 +1814,21 @@
         <v>3266133</v>
       </c>
       <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="8" t="s">
+      <c r="F22" t="s">
         <v>64</v>
       </c>
-      <c r="F22" t="s">
-        <v>65</v>
-      </c>
       <c r="G22" t="s">
-        <v>107</v>
-      </c>
-      <c r="H22">
+        <v>106</v>
+      </c>
+      <c r="H22" s="12">
         <v>65</v>
       </c>
     </row>
@@ -1781,21 +1837,21 @@
         <v>3265971</v>
       </c>
       <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F23" t="s">
-        <v>67</v>
-      </c>
       <c r="G23" t="s">
-        <v>107</v>
-      </c>
-      <c r="H23">
+        <v>106</v>
+      </c>
+      <c r="H23" s="9">
         <v>32.5</v>
       </c>
     </row>
@@ -1804,21 +1860,21 @@
         <v>3266023</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G24" t="s">
-        <v>107</v>
-      </c>
-      <c r="H24">
+        <v>106</v>
+      </c>
+      <c r="H24" s="9">
         <v>32.5</v>
       </c>
     </row>
@@ -1827,21 +1883,21 @@
         <v>3266265</v>
       </c>
       <c r="B25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="F25" t="s">
         <v>71</v>
       </c>
-      <c r="F25" t="s">
-        <v>72</v>
-      </c>
       <c r="G25" t="s">
-        <v>107</v>
-      </c>
-      <c r="H25">
+        <v>106</v>
+      </c>
+      <c r="H25" s="9">
         <v>32.5</v>
       </c>
     </row>
@@ -1850,21 +1906,21 @@
         <v>3266180</v>
       </c>
       <c r="B26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="D26" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>71</v>
-      </c>
       <c r="F26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G26" t="s">
-        <v>107</v>
-      </c>
-      <c r="H26">
+        <v>106</v>
+      </c>
+      <c r="H26" s="9">
         <v>32.5</v>
       </c>
     </row>
@@ -1873,25 +1929,25 @@
         <v>3266321</v>
       </c>
       <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="D27" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F27" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="G27" t="s">
+        <v>106</v>
+      </c>
+      <c r="H27" s="9">
+        <v>32.5</v>
+      </c>
+      <c r="J27" t="s">
         <v>109</v>
-      </c>
-      <c r="F27" t="s">
-        <v>76</v>
-      </c>
-      <c r="G27" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27">
-        <v>32.5</v>
-      </c>
-      <c r="J27" t="s">
-        <v>110</v>
       </c>
       <c r="K27">
         <v>40</v>
@@ -1902,21 +1958,21 @@
         <v>3265990</v>
       </c>
       <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>75</v>
-      </c>
       <c r="D28" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G28" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28">
+        <v>106</v>
+      </c>
+      <c r="H28" s="9">
         <v>32.5</v>
       </c>
     </row>
@@ -1930,4 +1986,817 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.453125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.90625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="25.26953125" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15">
+        <v>2663720</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="15">
+        <v>3037547</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="11">
+        <v>8382958</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="15">
+        <v>3067160</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="15">
+        <v>3265971</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="15">
+        <v>3266023</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="15">
+        <v>2949099</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="15">
+        <v>2652454</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="15">
+        <v>3266321</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" t="s">
+        <v>106</v>
+      </c>
+      <c r="H14">
+        <v>32.5</v>
+      </c>
+      <c r="J14" t="s">
+        <v>109</v>
+      </c>
+      <c r="K14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="15">
+        <v>3265990</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" t="s">
+        <v>106</v>
+      </c>
+      <c r="H15">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="15">
+        <v>3073191</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17">
+        <v>70</v>
+      </c>
+      <c r="J17" t="s">
+        <v>101</v>
+      </c>
+      <c r="K17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="15">
+        <v>3266265</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="15">
+        <v>3266180</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" t="s">
+        <v>106</v>
+      </c>
+      <c r="H20">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="15">
+        <v>3266324</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="11">
+        <v>1603687</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" t="s">
+        <v>106</v>
+      </c>
+      <c r="H22">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H24">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="15">
+        <v>3266106</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="11">
+        <v>3211863</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" t="s">
+        <v>106</v>
+      </c>
+      <c r="H26">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="34.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>3266133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2955619</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8">
+        <v>2181000</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>3266289</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10">
+        <v>1929525</v>
+      </c>
+      <c r="F10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H10">
+        <v>65</v>
+      </c>
+      <c r="K10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2657085</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>3037067</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14">
+        <v>3458347</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" t="s">
+        <v>99</v>
+      </c>
+      <c r="H14">
+        <v>70</v>
+      </c>
+      <c r="J14" t="s">
+        <v>105</v>
+      </c>
+      <c r="K14">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5"/>
+      <c r="G16" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C17" s="8"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2958822</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s">
+        <v>96</v>
+      </c>
+      <c r="H19">
+        <v>70</v>
+      </c>
+      <c r="J19" t="s">
+        <v>97</v>
+      </c>
+      <c r="K19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2951874</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" t="s">
+        <v>96</v>
+      </c>
+      <c r="H22">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2966414</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23">
+        <v>3628938</v>
+      </c>
+      <c r="F23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" t="s">
+        <v>96</v>
+      </c>
+      <c r="H23">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>